<commit_message>
Corrected input files upstream
</commit_message>
<xml_diff>
--- a/Fuels_case_input_test_20200302.xlsx
+++ b/Fuels_case_input_test_20200302.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/SEM-1.2_HOME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/truggles/SEM-1.2_CIW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863EAE5E-4BE9-F245-BFFB-3EEA8E978030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A77940-1201-3247-BB6B-51E3B193AE6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="-26080" windowWidth="28720" windowHeight="18520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_test_190726" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="212">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -636,18 +636,6 @@
     <t>EFFICIENCY_FUEL_ELECTROLYZER</t>
   </si>
   <si>
-    <t>Input_Data/SEM_TEMOA</t>
-  </si>
-  <si>
-    <t>SEM_TEMOA_demand.csv</t>
-  </si>
-  <si>
-    <t>SEM_TEMOA_solar.csv</t>
-  </si>
-  <si>
-    <t>SEM_TEMOA_wind.csv</t>
-  </si>
-  <si>
     <t>FUEL_DEMAND</t>
   </si>
   <si>
@@ -670,6 +658,21 @@
   </si>
   <si>
     <t>($/h)/kW (added to Electrolyzer b/c same scaling)</t>
+  </si>
+  <si>
+    <t>SYSTEM_RELIABILITY</t>
+  </si>
+  <si>
+    <t>Input_Data/Lei_Solar_Wind</t>
+  </si>
+  <si>
+    <t>US_demand_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_solar_25pctTop_unnormalized.csv</t>
+  </si>
+  <si>
+    <t>US_capacity_wind_25pctTop_unnormalized.csv</t>
   </si>
 </sst>
 </file>
@@ -1358,12 +1361,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR1031"/>
+  <dimension ref="A1:AU1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A146" sqref="A146"/>
-      <selection pane="topRight" activeCell="AN168" sqref="AN168"/>
+      <selection pane="topRight" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3079,7 +3082,7 @@
         <v>33</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>34</v>
@@ -3116,7 +3119,7 @@
         <v>35</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>36</v>
@@ -3582,7 +3585,7 @@
         <v>76</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
@@ -4082,7 +4085,7 @@
         <v>91</v>
       </c>
       <c r="B80" s="50" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="4"/>
@@ -4358,7 +4361,7 @@
         <v>167</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="4"/>
@@ -4634,7 +4637,7 @@
         <v>104</v>
       </c>
       <c r="B92" s="50" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -4910,7 +4913,7 @@
         <v>172</v>
       </c>
       <c r="B98" s="50" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -6950,7 +6953,7 @@
         <v>157</v>
       </c>
       <c r="B141" s="47" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="F141" s="8"/>
       <c r="H141" s="8"/>
@@ -7233,13 +7236,13 @@
     </row>
     <row r="150" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="70" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B150" s="67">
         <v>0</v>
       </c>
       <c r="C150" s="71" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F150" s="8"/>
       <c r="H150" s="8"/>
@@ -7273,7 +7276,7 @@
         <v>93</v>
       </c>
       <c r="D151" s="72" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F151" s="8"/>
       <c r="H151" s="8"/>
@@ -7461,14 +7464,14 @@
     </row>
     <row r="157" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="70" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B157" s="47">
         <v>0.68200000000000005</v>
       </c>
       <c r="C157" s="3"/>
       <c r="D157" s="71" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F157" s="8"/>
       <c r="H157" s="8"/>
@@ -7570,13 +7573,13 @@
     </row>
     <row r="160" spans="1:26" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="52" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B160" s="49">
         <v>1</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D160" s="69"/>
       <c r="E160" s="3"/>
@@ -7601,7 +7604,7 @@
       <c r="Y160" s="25"/>
       <c r="Z160" s="20"/>
     </row>
-    <row r="161" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:47" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="52"/>
       <c r="B161" s="47"/>
       <c r="C161" s="73"/>
@@ -7628,7 +7631,7 @@
       <c r="Y161" s="25"/>
       <c r="Z161" s="20"/>
     </row>
-    <row r="162" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:47" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="52"/>
       <c r="B162" s="47"/>
       <c r="F162" s="8"/>
@@ -7652,7 +7655,7 @@
       <c r="Y162" s="25"/>
       <c r="Z162" s="20"/>
     </row>
-    <row r="163" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="14" t="s">
         <v>145</v>
       </c>
@@ -7689,7 +7692,7 @@
       <c r="AB163" s="4"/>
       <c r="AC163" s="4"/>
     </row>
-    <row r="164" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="4"/>
@@ -7719,7 +7722,7 @@
       <c r="AB164" s="4"/>
       <c r="AC164" s="4"/>
     </row>
-    <row r="165" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
       <c r="B165" s="4"/>
       <c r="C165" s="3" t="s">
@@ -7752,7 +7755,7 @@
       <c r="AB165" s="4"/>
       <c r="AC165" s="4"/>
     </row>
-    <row r="166" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3"/>
       <c r="B166" s="4"/>
       <c r="C166" s="3"/>
@@ -7783,7 +7786,7 @@
       <c r="AB166" s="4"/>
       <c r="AC166" s="4"/>
     </row>
-    <row r="167" spans="1:44" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:47" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="54" t="s">
         <v>147</v>
       </c>
@@ -7791,7 +7794,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="168" spans="1:44" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:47" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A168" s="44" t="s">
         <v>149</v>
       </c>
@@ -7907,25 +7910,34 @@
         <v>154</v>
       </c>
       <c r="AM168" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN168" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="AN168" s="51" t="s">
+      <c r="AO168" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="AO168" s="44" t="s">
+      <c r="AP168" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="AP168" s="44" t="s">
+      <c r="AQ168" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="AQ168" s="44" t="s">
+      <c r="AR168" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="AR168" s="44" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="169" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AS168" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="AT168" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="AU168" s="44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="169" spans="1:47" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B169" s="55"/>
       <c r="C169" s="55"/>
       <c r="D169" s="55"/>
@@ -7966,7 +7978,7 @@
       <c r="AM169" s="55"/>
       <c r="AN169" s="55"/>
     </row>
-    <row r="170" spans="1:44" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:47" s="59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="56" t="s">
         <v>184</v>
       </c>
@@ -8082,10 +8094,10 @@
         <v>1</v>
       </c>
       <c r="AM170" s="57">
+        <v>1</v>
+      </c>
+      <c r="AN170" s="57">
         <v>-1</v>
-      </c>
-      <c r="AN170" s="57">
-        <v>1</v>
       </c>
       <c r="AO170" s="56">
         <v>1</v>
@@ -8094,22 +8106,31 @@
         <v>1</v>
       </c>
       <c r="AQ170" s="59">
+        <v>1</v>
+      </c>
+      <c r="AR170" s="59">
         <v>0</v>
       </c>
-      <c r="AR170" s="59">
+      <c r="AS170" s="59">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:44" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AT170" s="59">
+        <v>1</v>
+      </c>
+      <c r="AU170" s="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:47" s="53" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B171" s="45"/>
     </row>
-    <row r="172" spans="1:44" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:47" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="54" t="s">
         <v>150</v>
       </c>
       <c r="B172" s="43"/>
     </row>
-    <row r="173" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3"/>
       <c r="B173" s="4"/>
       <c r="C173" s="3"/>
@@ -8140,7 +8161,7 @@
       <c r="AB173" s="4"/>
       <c r="AC173" s="4"/>
     </row>
-    <row r="174" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3"/>
       <c r="B174" s="4"/>
       <c r="C174" s="3"/>
@@ -8171,7 +8192,7 @@
       <c r="AB174" s="4"/>
       <c r="AC174" s="4"/>
     </row>
-    <row r="175" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3"/>
       <c r="B175" s="4"/>
       <c r="C175" s="3"/>
@@ -8202,7 +8223,7 @@
       <c r="AB175" s="4"/>
       <c r="AC175" s="4"/>
     </row>
-    <row r="176" spans="1:44" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3"/>
       <c r="B176" s="4"/>
       <c r="C176" s="3"/>

</xml_diff>